<commit_message>
[Mod] Tileinfo, Data 수정
</commit_message>
<xml_diff>
--- a/Assets/10.Data/ItemCombinationDataTable.xlsx
+++ b/Assets/10.Data/ItemCombinationDataTable.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceTree\Project_60Days\Assets\10.Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Project_60Days\Assets\10.Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC8FD26-CA43-4104-894D-3324B61D2071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12870"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>인덱스</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,10 +47,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ITEM_TIER_1_METAL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>강판</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -110,14 +107,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ITEM_TIER_1_METAL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ITEM_TIER_1_METAL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>재료7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -131,13 +120,17 @@
   </si>
   <si>
     <t>Material_8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEM_TIER_1_PLATE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -241,7 +234,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -252,12 +245,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -554,11 +541,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -571,193 +558,193 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>25</v>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3">
         <v>1001</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="4">
+      <c r="D3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="3">
         <v>-1</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>-1</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>-1</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>-1</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>-1</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <v>-1</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
         <v>1002</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
         <v>1003</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
         <v>1004</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
         <v>1005</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
         <v>1006</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -766,14 +753,14 @@
       <c r="C9" s="3">
         <v>1007</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -782,14 +769,14 @@
       <c r="C10" s="3">
         <v>1008</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -798,14 +785,14 @@
       <c r="C11" s="3">
         <v>1009</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -814,14 +801,14 @@
       <c r="C12" s="3">
         <v>1010</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -830,14 +817,14 @@
       <c r="C13" s="3">
         <v>1011</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -846,14 +833,14 @@
       <c r="C14" s="3">
         <v>1012</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -862,14 +849,14 @@
       <c r="C15" s="3">
         <v>1013</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -878,14 +865,14 @@
       <c r="C16" s="3">
         <v>1014</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -894,14 +881,14 @@
       <c r="C17" s="3">
         <v>1015</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -910,14 +897,14 @@
       <c r="C18" s="3">
         <v>1016</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -926,14 +913,14 @@
       <c r="C19" s="3">
         <v>1017</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -942,14 +929,14 @@
       <c r="C20" s="3">
         <v>1018</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -958,14 +945,14 @@
       <c r="C21" s="3">
         <v>1019</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -974,14 +961,14 @@
       <c r="C22" s="3">
         <v>1020</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -990,14 +977,14 @@
       <c r="C23" s="3">
         <v>1021</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -1006,14 +993,14 @@
       <c r="C24" s="3">
         <v>1022</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -1022,14 +1009,14 @@
       <c r="C25" s="3">
         <v>1023</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -1038,14 +1025,14 @@
       <c r="C26" s="3">
         <v>1024</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -1054,14 +1041,14 @@
       <c r="C27" s="3">
         <v>1025</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -1070,14 +1057,14 @@
       <c r="C28" s="3">
         <v>1026</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -1086,14 +1073,14 @@
       <c r="C29" s="3">
         <v>1027</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -1102,14 +1089,14 @@
       <c r="C30" s="3">
         <v>1028</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -1118,14 +1105,14 @@
       <c r="C31" s="3">
         <v>1029</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -1134,14 +1121,14 @@
       <c r="C32" s="3">
         <v>1030</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -1150,14 +1137,14 @@
       <c r="C33" s="3">
         <v>1031</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
   </sheetData>

</xml_diff>